<commit_message>
feat(translation): add all translation files to script location
</commit_message>
<xml_diff>
--- a/utils/localisation_script/excel_to_json/as/Assamese - Generic DELTA.xlsx
+++ b/utils/localisation_script/excel_to_json/as/Assamese - Generic DELTA.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localisation_script/excel_to_json/as/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606C9CD3-4721-FD4E-BA10-C9CCED1F0C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delta" sheetId="7" r:id="rId1"/>
@@ -183,7 +189,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-5000445]0"/>
   </numFmts>
@@ -525,64 +531,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" style="6"/>
+    <col min="1" max="2" width="14.5" style="6"/>
     <col min="3" max="3" width="21" style="6" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="51.140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="6"/>
-    <col min="7" max="7" width="57.5703125" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="14.42578125" style="6"/>
+    <col min="4" max="4" width="21.1640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="51.1640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="6"/>
+    <col min="7" max="7" width="57.5" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="14.5" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:7" ht="15">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="5" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25.5">
-      <c r="A3" s="7" t="s">
+    <row r="4" spans="1:7" ht="28">
+      <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="D4" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>17</v>
@@ -591,201 +586,212 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="D5" s="8" t="s">
+    <row r="5" spans="1:7" ht="14">
+      <c r="D5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14">
+      <c r="D6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="89.25">
-      <c r="D6" s="8" t="s">
+    <row r="7" spans="1:7" ht="98">
+      <c r="D7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="E7" s="3"/>
-    </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="7" t="s">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="14">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="25.5">
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="14">
+      <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
     <row r="11" spans="1:7">
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="14">
+      <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E12" s="9">
         <v>1</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G12" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="89.25">
-      <c r="C12" s="7"/>
-      <c r="D12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="98">
       <c r="C13" s="7"/>
       <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14">
+      <c r="C14" s="7"/>
+      <c r="D14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="C14" s="2" t="s">
+    <row r="15" spans="1:7" ht="14">
+      <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E15" s="11">
         <v>2</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G15" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="89.25">
-      <c r="C15" s="7"/>
-      <c r="D15" s="12" t="s">
+    <row r="16" spans="1:7" ht="98">
+      <c r="C16" s="7"/>
+      <c r="D16" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G16" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="C16" s="7"/>
-      <c r="D16" s="2" t="s">
+    <row r="17" spans="3:7" ht="14">
+      <c r="C17" s="7"/>
+      <c r="D17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="3:7">
-      <c r="C17" s="2" t="s">
+    <row r="18" spans="3:7" ht="14">
+      <c r="C18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E18" s="9">
         <v>3</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G18" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="3:7" ht="76.5">
-      <c r="C18" s="7"/>
-      <c r="D18" s="12" t="s">
+    <row r="19" spans="3:7" ht="84">
+      <c r="C19" s="7"/>
+      <c r="D19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G19" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="3:7">
-      <c r="C19" s="7"/>
-      <c r="D19" s="2" t="s">
+    <row r="20" spans="3:7" ht="14">
+      <c r="C20" s="7"/>
+      <c r="D20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="3:7">
-      <c r="C20" s="2" t="s">
+    <row r="21" spans="3:7" ht="14">
+      <c r="C21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E21" s="9">
         <v>4</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G21" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:7" ht="102">
-      <c r="C21" s="7"/>
-      <c r="D21" s="12" t="s">
+    <row r="22" spans="3:7" ht="112">
+      <c r="C22" s="7"/>
+      <c r="D22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G22" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="3:7">
-      <c r="C22" s="7"/>
-      <c r="D22" s="2" t="s">
+    <row r="23" spans="3:7" ht="14">
+      <c r="C23" s="7"/>
+      <c r="D23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>